<commit_message>
Enable text wrapping for question label
</commit_message>
<xml_diff>
--- a/MathTutor/questions/question.xlsx
+++ b/MathTutor/questions/question.xlsx
@@ -124,13 +124,13 @@
     <t xml:space="preserve">a10:25*b5:15*</t>
   </si>
   <si>
-    <t xml:space="preserve">A train is {a} meters long and crosses a bridge {b} meters long. What is the total distance covered by the train while crossing the bridge?distance</t>
+    <t xml:space="preserve">A train is {a} meters long and crosses a bridge {b} meters long. What is the total distance covered by the train while crossing the bridge?</t>
   </si>
   <si>
     <t xml:space="preserve">a200,250*b150,200*</t>
   </si>
   <si>
-    <t xml:space="preserve">A delivery truck is {a} kilometers from its destination. It travels {b} kilometers in one hour. How much distance is left to cover after one hour?"</t>
+    <t xml:space="preserve">A delivery truck is {a} kilometers from its destination. It travels {b} kilometers in one hour. How much distance is left to cover after one hour?</t>
   </si>
   <si>
     <t xml:space="preserve">a150:200*b40:50*</t>
@@ -236,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -266,12 +266,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -315,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -325,10 +319,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,10 +346,10 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="107.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -768,7 +758,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -788,7 +778,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -808,7 +798,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -828,7 +818,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="0" t="s">

</xml_diff>